<commit_message>
Enhance department management and error handling: update delete department logic to check for assigned positions, improve error messages for department deletion, and add a debug route for department details. Refactor user permissions handling in user routes for better session management.
</commit_message>
<xml_diff>
--- a/static/templates/employee_template.xlsx
+++ b/static/templates/employee_template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Business ID</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>is_active</t>
+  </si>
+  <si>
+    <t>hire_date</t>
   </si>
 </sst>
 </file>
@@ -59,7 +62,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border/>
     <border>
       <left style="thin">
@@ -119,6 +122,34 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF6F8F9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF6F8F9"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
@@ -126,6 +157,20 @@
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF6F8F9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -135,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -160,16 +205,25 @@
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -230,8 +284,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G11" displayName="Tableau1" name="Tableau1" id="1">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H11" displayName="Tableau1" name="Tableau1" id="1">
+  <tableColumns count="8">
     <tableColumn name="Business ID" id="1"/>
     <tableColumn name="English Name" id="2"/>
     <tableColumn name="Arabic Name" id="3"/>
@@ -239,6 +293,7 @@
     <tableColumn name="Phone" id="5"/>
     <tableColumn name="Departments" id="6"/>
     <tableColumn name="is_active" id="7"/>
+    <tableColumn name="hire_date" id="8"/>
   </tableColumns>
   <tableStyleInfo name="Feuille 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -457,6 +512,7 @@
     <col customWidth="1" min="4" max="4" width="19.5"/>
     <col customWidth="1" min="5" max="5" width="13.5"/>
     <col customWidth="1" min="6" max="7" width="15.13"/>
+    <col customWidth="1" min="8" max="8" width="15.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -478,8 +534,11 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2">
@@ -490,6 +549,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="4"/>
       <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="4"/>
@@ -499,6 +559,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="4"/>
       <c r="G3" s="7"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4">
       <c r="A4" s="4"/>
@@ -508,6 +569,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" s="4"/>
@@ -517,6 +579,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="4"/>
       <c r="G5" s="7"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6">
       <c r="A6" s="4"/>
@@ -526,6 +589,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="4"/>
       <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7">
       <c r="A7" s="4"/>
@@ -535,6 +599,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="4"/>
       <c r="G7" s="7"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8">
       <c r="A8" s="4"/>
@@ -544,6 +609,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="4"/>
       <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="4"/>
@@ -553,6 +619,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="4"/>
       <c r="G9" s="7"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10">
       <c r="A10" s="4"/>
@@ -562,15 +629,17 @@
       <c r="E10" s="6"/>
       <c r="F10" s="4"/>
       <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -580,6 +649,7 @@
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:E11">
       <formula1>AND(ISNUMBER(E2),(NOT(OR(NOT(ISERROR(DATEVALUE(E2))), AND(ISNUMBER(E2), LEFT(CELL("format", E2))="D")))))</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="H2:H11"/>
   </dataValidations>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>